<commit_message>
Clarifying the use of terms
</commit_message>
<xml_diff>
--- a/Literature_data_template.xlsx
+++ b/Literature_data_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b521975c2e27c04/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SBolshakov\GoogleDrive\BDI\Literature_data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44833FF6-7A1A-42ED-9913-57DDCECE7719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8F9F5C-58CD-45A7-A941-E947209F0F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27780" windowHeight="16440" xr2:uid="{F2D4E312-E302-4068-BA5D-D116D593F785}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>associatedReferences</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>verbatimLongitude</t>
+  </si>
+  <si>
+    <t>bibliographicCitation</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA532AB-53C8-4BD1-A8D7-67CFD2D789BE}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -480,17 +483,17 @@
   <cols>
     <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="20.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="2" customWidth="1"/>
-    <col min="8" max="10" width="20.7109375" style="2" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" style="2" customWidth="1"/>
-    <col min="13" max="24" width="20.7109375" style="2" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="4" width="20.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="10" width="20.7109375" style="2" customWidth="1"/>
+    <col min="11" max="13" width="10.7109375" style="2" customWidth="1"/>
+    <col min="14" max="25" width="20.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -499,66 +502,69 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>